<commit_message>
validacion de detalle de paleta en los kilos netos y brutos
</commit_message>
<xml_diff>
--- a/bin/Debug/net9.0-windows/detalle_paleta.xlsx
+++ b/bin/Debug/net9.0-windows/detalle_paleta.xlsx
@@ -34,28 +34,18 @@
     <x:t>Kilo_Bruto</x:t>
   </x:si>
   <x:si>
-    <x:t>9</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1000</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">50x50     </x:t>
-  </x:si>
-  <x:si>
-    <x:t>150 ROLLOS 4X5000
-100 ROLLOS 5X5000
-150 HOJAS
-150 GRAPHICS</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1001</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">48X48     </x:t>
-  </x:si>
-  <x:si>
-    <x:t>300 ROLLOS 5 5500</x:t>
+    <x:t>45</x:t>
+  </x:si>
+  <x:si>
+    <x:t>69</x:t>
+  </x:si>
+  <x:si>
+    <x:t>50X50</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DFNSA.FSFSDFJÑKÑ.KSAJFH
+SF-SHFKJSHFÑKSADJFSÑKJFH
+SDLFKHSLFKSÑAFHASDÑF</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -425,7 +415,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:F3"/>
+  <x:dimension ref="A1:F2"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -433,8 +423,8 @@
   <x:cols>
     <x:col min="1" max="1" width="8.282054" style="0" customWidth="1"/>
     <x:col min="2" max="2" width="13.853482" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="8.567768" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="18.567768" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="7.853482" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="26.139196" style="0" customWidth="1"/>
     <x:col min="5" max="5" width="9.567768" style="0" customWidth="1"/>
     <x:col min="6" max="6" width="10.282054" style="0" customWidth="1"/>
   </x:cols>
@@ -473,30 +463,10 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="E2" s="0">
-        <x:v>1280</x:v>
+        <x:v>850</x:v>
       </x:c>
       <x:c r="F2" s="0">
-        <x:v>1388</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:6">
-      <x:c r="A3" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="B3" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="C3" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="D3" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="E3" s="0">
-        <x:v>1000</x:v>
-      </x:c>
-      <x:c r="F3" s="0">
-        <x:v>1100</x:v>
+        <x:v>1250</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>